<commit_message>
Finalización de la prueba
</commit_message>
<xml_diff>
--- a/punto_1/resultado.xlsx
+++ b/punto_1/resultado.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eafit-my.sharepoint.com/personal/scarmonae_eafit_edu_co/Documents/REPOSITORIOS/Test_Dataknow/punto_1/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_016D43F4071B0C39692C4C39DD6B1A0B787C240D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B26EB82-675E-4D96-9219-B39A1D0D1468}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -1639,8 +1633,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1703,21 +1697,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1755,7 +1741,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1789,7 +1775,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1824,10 +1809,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2000,22 +1984,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AA306"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="19.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
-    <col min="4" max="12" width="6.90625" bestFit="1" customWidth="1"/>
-    <col min="13" max="27" width="7.90625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:27">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2095,7 +2071,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:27">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2178,7 +2154,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:27">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -2261,7 +2237,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:27">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -2344,7 +2320,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:27">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -2427,7 +2403,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:27">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -2510,7 +2486,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:27">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -2593,7 +2569,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:27">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -2676,7 +2652,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:27">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -2759,7 +2735,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:27">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -2842,7 +2818,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:27">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -2925,7 +2901,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:27">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -3008,7 +2984,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:27">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -3091,7 +3067,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:27">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -3174,7 +3150,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:27">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -3257,7 +3233,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:27">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -3340,7 +3316,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:27">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -3423,7 +3399,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:27">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -3506,7 +3482,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:27">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -3589,7 +3565,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:27">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -3672,7 +3648,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:27">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -3755,7 +3731,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:27">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -3838,7 +3814,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:27">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -3921,7 +3897,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:27">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -4004,7 +3980,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:27">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -4087,7 +4063,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:27">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -4170,7 +4146,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:27">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -4253,7 +4229,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:27">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -4336,7 +4312,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:27">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -4419,7 +4395,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:27">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -4502,7 +4478,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:27">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -4585,7 +4561,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:27">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -4668,7 +4644,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:27">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -4751,7 +4727,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:27">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -4834,7 +4810,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:27">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -4917,7 +4893,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:27">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -5000,7 +4976,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:27">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -5083,7 +5059,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:27">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -5166,7 +5142,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:27">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -5249,7 +5225,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:27">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -5332,7 +5308,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:27">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -5415,7 +5391,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:27">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -5498,7 +5474,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:27">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -5581,7 +5557,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="44" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:27">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -5664,7 +5640,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="45" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:27">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -5747,7 +5723,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="46" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:27">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -5830,7 +5806,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="47" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:27">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -5913,7 +5889,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="48" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:27">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -5996,7 +5972,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="49" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:27">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -6079,7 +6055,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="50" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:27">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -6162,7 +6138,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="51" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:27">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -6245,7 +6221,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="52" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:27">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -6328,7 +6304,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="53" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:27">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -6411,7 +6387,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="54" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:27">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -6494,7 +6470,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="55" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:27">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -6577,7 +6553,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="56" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:27">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -6660,7 +6636,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="57" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:27">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -6743,7 +6719,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="58" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:27">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -6826,7 +6802,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="59" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:27">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -6909,7 +6885,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="60" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:27">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -6992,7 +6968,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="61" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:27">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -7075,7 +7051,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="62" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:27">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -7158,7 +7134,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="63" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:27">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -7241,7 +7217,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="64" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:27">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -7324,7 +7300,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="65" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:27">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -7407,7 +7383,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="66" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:27">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -7490,7 +7466,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="67" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:27">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -7573,7 +7549,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="68" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:27">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -7656,7 +7632,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="69" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:27">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -7739,7 +7715,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="70" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:27">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -7822,7 +7798,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="71" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:27">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -7905,7 +7881,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="72" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:27">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -7988,7 +7964,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="73" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:27">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -8071,7 +8047,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="74" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:27">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -8154,7 +8130,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="75" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:27">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -8237,7 +8213,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="76" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:27">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -8320,7 +8296,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="77" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:27">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -8403,7 +8379,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="78" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:27">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -8486,7 +8462,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="79" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:27">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -8569,7 +8545,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="80" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:27">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -8652,7 +8628,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="81" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:27">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -8735,7 +8711,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="82" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:27">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -8818,7 +8794,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="83" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:27">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -8901,7 +8877,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="84" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:27">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -8984,7 +8960,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="85" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:27">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -9067,7 +9043,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="86" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:27">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -9150,7 +9126,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="87" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:27">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -9233,7 +9209,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="88" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:27">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -9316,7 +9292,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="89" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:27">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -9399,7 +9375,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="90" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:27">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -9482,7 +9458,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="91" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:27">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -9565,7 +9541,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="92" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:27">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -9648,7 +9624,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="93" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:27">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -9731,7 +9707,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="94" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:27">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -9814,7 +9790,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="95" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:27">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -9897,7 +9873,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="96" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:27">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -9980,7 +9956,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="97" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:27">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -10063,7 +10039,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="98" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:27">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -10146,7 +10122,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="99" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:27">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -10229,7 +10205,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="100" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:27">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -10312,7 +10288,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="101" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:27">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -10395,7 +10371,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="102" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:27">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -10478,7 +10454,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="103" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:27">
       <c r="A103" s="1">
         <v>101</v>
       </c>
@@ -10561,7 +10537,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="104" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:27">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -10644,7 +10620,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="105" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:27">
       <c r="A105" s="1">
         <v>103</v>
       </c>
@@ -10727,7 +10703,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="106" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:27">
       <c r="A106" s="1">
         <v>104</v>
       </c>
@@ -10810,7 +10786,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="107" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:27">
       <c r="A107" s="1">
         <v>105</v>
       </c>
@@ -10893,7 +10869,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="108" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:27">
       <c r="A108" s="1">
         <v>106</v>
       </c>
@@ -10976,7 +10952,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="109" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:27">
       <c r="A109" s="1">
         <v>107</v>
       </c>
@@ -11059,7 +11035,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="110" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:27">
       <c r="A110" s="1">
         <v>108</v>
       </c>
@@ -11142,7 +11118,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="111" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:27">
       <c r="A111" s="1">
         <v>109</v>
       </c>
@@ -11225,7 +11201,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="112" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:27">
       <c r="A112" s="1">
         <v>110</v>
       </c>
@@ -11308,7 +11284,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="113" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:27">
       <c r="A113" s="1">
         <v>111</v>
       </c>
@@ -11391,7 +11367,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="114" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:27">
       <c r="A114" s="1">
         <v>112</v>
       </c>
@@ -11474,7 +11450,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="115" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:27">
       <c r="A115" s="1">
         <v>113</v>
       </c>
@@ -11557,7 +11533,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="116" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:27">
       <c r="A116" s="1">
         <v>114</v>
       </c>
@@ -11640,7 +11616,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="117" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:27">
       <c r="A117" s="1">
         <v>115</v>
       </c>
@@ -11723,7 +11699,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="118" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:27">
       <c r="A118" s="1">
         <v>116</v>
       </c>
@@ -11806,7 +11782,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="119" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:27">
       <c r="A119" s="1">
         <v>117</v>
       </c>
@@ -11889,7 +11865,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="120" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:27">
       <c r="A120" s="1">
         <v>118</v>
       </c>
@@ -11972,7 +11948,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="121" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:27">
       <c r="A121" s="1">
         <v>119</v>
       </c>
@@ -12055,7 +12031,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="122" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:27">
       <c r="A122" s="1">
         <v>120</v>
       </c>
@@ -12138,7 +12114,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="123" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:27">
       <c r="A123" s="1">
         <v>121</v>
       </c>
@@ -12221,7 +12197,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="124" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:27">
       <c r="A124" s="1">
         <v>122</v>
       </c>
@@ -12304,7 +12280,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="125" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:27">
       <c r="A125" s="1">
         <v>123</v>
       </c>
@@ -12387,7 +12363,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="126" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:27">
       <c r="A126" s="1">
         <v>124</v>
       </c>
@@ -12470,7 +12446,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="127" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:27">
       <c r="A127" s="1">
         <v>125</v>
       </c>
@@ -12553,7 +12529,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="128" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:27">
       <c r="A128" s="1">
         <v>126</v>
       </c>
@@ -12636,7 +12612,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="129" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:27">
       <c r="A129" s="1">
         <v>127</v>
       </c>
@@ -12719,7 +12695,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="130" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:27">
       <c r="A130" s="1">
         <v>128</v>
       </c>
@@ -12802,7 +12778,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="131" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:27">
       <c r="A131" s="1">
         <v>129</v>
       </c>
@@ -12885,7 +12861,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="132" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:27">
       <c r="A132" s="1">
         <v>130</v>
       </c>
@@ -12968,7 +12944,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="133" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:27">
       <c r="A133" s="1">
         <v>131</v>
       </c>
@@ -13051,7 +13027,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="134" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:27">
       <c r="A134" s="1">
         <v>132</v>
       </c>
@@ -13134,7 +13110,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="135" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:27">
       <c r="A135" s="1">
         <v>133</v>
       </c>
@@ -13217,7 +13193,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="136" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:27">
       <c r="A136" s="1">
         <v>134</v>
       </c>
@@ -13300,7 +13276,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="137" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:27">
       <c r="A137" s="1">
         <v>135</v>
       </c>
@@ -13383,7 +13359,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="138" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:27">
       <c r="A138" s="1">
         <v>136</v>
       </c>
@@ -13466,7 +13442,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="139" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:27">
       <c r="A139" s="1">
         <v>137</v>
       </c>
@@ -13549,7 +13525,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="140" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:27">
       <c r="A140" s="1">
         <v>138</v>
       </c>
@@ -13632,7 +13608,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="141" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:27">
       <c r="A141" s="1">
         <v>139</v>
       </c>
@@ -13715,7 +13691,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="142" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:27">
       <c r="A142" s="1">
         <v>140</v>
       </c>
@@ -13798,7 +13774,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="143" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:27">
       <c r="A143" s="1">
         <v>141</v>
       </c>
@@ -13881,7 +13857,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="144" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:27">
       <c r="A144" s="1">
         <v>142</v>
       </c>
@@ -13964,7 +13940,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="145" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:27">
       <c r="A145" s="1">
         <v>143</v>
       </c>
@@ -14047,7 +14023,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="146" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:27">
       <c r="A146" s="1">
         <v>144</v>
       </c>
@@ -14130,7 +14106,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="147" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:27">
       <c r="A147" s="1">
         <v>145</v>
       </c>
@@ -14213,7 +14189,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="148" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:27">
       <c r="A148" s="1">
         <v>146</v>
       </c>
@@ -14296,7 +14272,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="149" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:27">
       <c r="A149" s="1">
         <v>147</v>
       </c>
@@ -14379,7 +14355,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="150" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:27">
       <c r="A150" s="1">
         <v>148</v>
       </c>
@@ -14462,7 +14438,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="151" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:27">
       <c r="A151" s="1">
         <v>149</v>
       </c>
@@ -14545,7 +14521,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="152" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:27">
       <c r="A152" s="1">
         <v>150</v>
       </c>
@@ -14628,7 +14604,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="153" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:27">
       <c r="A153" s="1">
         <v>151</v>
       </c>
@@ -14711,7 +14687,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="154" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:27">
       <c r="A154" s="1">
         <v>152</v>
       </c>
@@ -14794,7 +14770,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="155" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:27">
       <c r="A155" s="1">
         <v>153</v>
       </c>
@@ -14877,7 +14853,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="156" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:27">
       <c r="A156" s="1">
         <v>154</v>
       </c>
@@ -14960,7 +14936,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="157" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:27">
       <c r="A157" s="1">
         <v>155</v>
       </c>
@@ -15043,7 +15019,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="158" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:27">
       <c r="A158" s="1">
         <v>156</v>
       </c>
@@ -15126,7 +15102,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="159" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:27">
       <c r="A159" s="1">
         <v>157</v>
       </c>
@@ -15209,7 +15185,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="160" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:27">
       <c r="A160" s="1">
         <v>158</v>
       </c>
@@ -15292,7 +15268,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="161" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:27">
       <c r="A161" s="1">
         <v>159</v>
       </c>
@@ -15375,7 +15351,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="162" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:27">
       <c r="A162" s="1">
         <v>160</v>
       </c>
@@ -15458,7 +15434,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="163" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:27">
       <c r="A163" s="1">
         <v>161</v>
       </c>
@@ -15541,7 +15517,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="164" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:27">
       <c r="A164" s="1">
         <v>162</v>
       </c>
@@ -15624,7 +15600,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="165" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:27">
       <c r="A165" s="1">
         <v>163</v>
       </c>
@@ -15707,7 +15683,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="166" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:27">
       <c r="A166" s="1">
         <v>164</v>
       </c>
@@ -15790,7 +15766,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="167" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:27">
       <c r="A167" s="1">
         <v>165</v>
       </c>
@@ -15873,7 +15849,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="168" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:27">
       <c r="A168" s="1">
         <v>166</v>
       </c>
@@ -15956,7 +15932,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="169" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:27">
       <c r="A169" s="1">
         <v>167</v>
       </c>
@@ -16039,7 +16015,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="170" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:27">
       <c r="A170" s="1">
         <v>168</v>
       </c>
@@ -16122,7 +16098,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="171" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:27">
       <c r="A171" s="1">
         <v>169</v>
       </c>
@@ -16205,7 +16181,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="172" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:27">
       <c r="A172" s="1">
         <v>170</v>
       </c>
@@ -16288,7 +16264,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="173" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:27">
       <c r="A173" s="1">
         <v>171</v>
       </c>
@@ -16371,7 +16347,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="174" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:27">
       <c r="A174" s="1">
         <v>172</v>
       </c>
@@ -16454,7 +16430,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="175" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:27">
       <c r="A175" s="1">
         <v>173</v>
       </c>
@@ -16537,7 +16513,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="176" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:27">
       <c r="A176" s="1">
         <v>174</v>
       </c>
@@ -16620,7 +16596,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="177" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:27">
       <c r="A177" s="1">
         <v>175</v>
       </c>
@@ -16703,7 +16679,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="178" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:27">
       <c r="A178" s="1">
         <v>176</v>
       </c>
@@ -16786,7 +16762,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="179" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:27">
       <c r="A179" s="1">
         <v>177</v>
       </c>
@@ -16869,7 +16845,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="180" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:27">
       <c r="A180" s="1">
         <v>178</v>
       </c>
@@ -16952,7 +16928,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="181" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:27">
       <c r="A181" s="1">
         <v>179</v>
       </c>
@@ -17035,7 +17011,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="182" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:27">
       <c r="A182" s="1">
         <v>180</v>
       </c>
@@ -17118,7 +17094,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="183" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:27">
       <c r="A183" s="1">
         <v>181</v>
       </c>
@@ -17201,7 +17177,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="184" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:27">
       <c r="A184" s="1">
         <v>182</v>
       </c>
@@ -17284,7 +17260,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="185" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:27">
       <c r="A185" s="1">
         <v>183</v>
       </c>
@@ -17367,7 +17343,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="186" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:27">
       <c r="A186" s="1">
         <v>184</v>
       </c>
@@ -17450,7 +17426,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="187" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:27">
       <c r="A187" s="1">
         <v>185</v>
       </c>
@@ -17533,7 +17509,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="188" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:27">
       <c r="A188" s="1">
         <v>186</v>
       </c>
@@ -17616,7 +17592,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="189" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:27">
       <c r="A189" s="1">
         <v>187</v>
       </c>
@@ -17699,7 +17675,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="190" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:27">
       <c r="A190" s="1">
         <v>188</v>
       </c>
@@ -17782,7 +17758,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="191" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:27">
       <c r="A191" s="1">
         <v>189</v>
       </c>
@@ -17865,7 +17841,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="192" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:27">
       <c r="A192" s="1">
         <v>190</v>
       </c>
@@ -17948,7 +17924,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="193" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:27">
       <c r="A193" s="1">
         <v>191</v>
       </c>
@@ -18031,7 +18007,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="194" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:27">
       <c r="A194" s="1">
         <v>192</v>
       </c>
@@ -18114,7 +18090,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="195" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:27">
       <c r="A195" s="1">
         <v>193</v>
       </c>
@@ -18197,7 +18173,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="196" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:27">
       <c r="A196" s="1">
         <v>194</v>
       </c>
@@ -18280,7 +18256,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="197" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:27">
       <c r="A197" s="1">
         <v>195</v>
       </c>
@@ -18363,7 +18339,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="198" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:27">
       <c r="A198" s="1">
         <v>196</v>
       </c>
@@ -18446,7 +18422,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="199" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:27">
       <c r="A199" s="1">
         <v>197</v>
       </c>
@@ -18529,7 +18505,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="200" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:27">
       <c r="A200" s="1">
         <v>198</v>
       </c>
@@ -18612,7 +18588,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="201" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:27">
       <c r="A201" s="1">
         <v>199</v>
       </c>
@@ -18695,7 +18671,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="202" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:27">
       <c r="A202" s="1">
         <v>200</v>
       </c>
@@ -18778,7 +18754,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="203" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:27">
       <c r="A203" s="1">
         <v>201</v>
       </c>
@@ -18861,7 +18837,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="204" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:27">
       <c r="A204" s="1">
         <v>202</v>
       </c>
@@ -18944,7 +18920,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="205" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:27">
       <c r="A205" s="1">
         <v>203</v>
       </c>
@@ -19027,7 +19003,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="206" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:27">
       <c r="A206" s="1">
         <v>204</v>
       </c>
@@ -19110,7 +19086,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="207" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:27">
       <c r="A207" s="1">
         <v>205</v>
       </c>
@@ -19193,7 +19169,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="208" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:27">
       <c r="A208" s="1">
         <v>206</v>
       </c>
@@ -19276,7 +19252,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="209" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:27">
       <c r="A209" s="1">
         <v>207</v>
       </c>
@@ -19359,7 +19335,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="210" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:27">
       <c r="A210" s="1">
         <v>208</v>
       </c>
@@ -19442,7 +19418,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="211" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:27">
       <c r="A211" s="1">
         <v>209</v>
       </c>
@@ -19525,7 +19501,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="212" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:27">
       <c r="A212" s="1">
         <v>210</v>
       </c>
@@ -19608,7 +19584,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="213" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:27">
       <c r="A213" s="1">
         <v>211</v>
       </c>
@@ -19691,7 +19667,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="214" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:27">
       <c r="A214" s="1">
         <v>212</v>
       </c>
@@ -19774,7 +19750,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="215" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:27">
       <c r="A215" s="1">
         <v>213</v>
       </c>
@@ -19857,7 +19833,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="216" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:27">
       <c r="A216" s="1">
         <v>214</v>
       </c>
@@ -19940,7 +19916,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="217" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:27">
       <c r="A217" s="1">
         <v>215</v>
       </c>
@@ -20023,7 +19999,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="218" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:27">
       <c r="A218" s="1">
         <v>216</v>
       </c>
@@ -20106,7 +20082,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="219" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:27">
       <c r="A219" s="1">
         <v>217</v>
       </c>
@@ -20189,7 +20165,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="220" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:27">
       <c r="A220" s="1">
         <v>218</v>
       </c>
@@ -20272,7 +20248,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="221" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:27">
       <c r="A221" s="1">
         <v>219</v>
       </c>
@@ -20355,7 +20331,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="222" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:27">
       <c r="A222" s="1">
         <v>220</v>
       </c>
@@ -20438,7 +20414,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="223" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:27">
       <c r="A223" s="1">
         <v>221</v>
       </c>
@@ -20521,7 +20497,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="224" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:27">
       <c r="A224" s="1">
         <v>222</v>
       </c>
@@ -20604,7 +20580,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="225" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:27">
       <c r="A225" s="1">
         <v>223</v>
       </c>
@@ -20687,7 +20663,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="226" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:27">
       <c r="A226" s="1">
         <v>224</v>
       </c>
@@ -20770,7 +20746,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="227" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:27">
       <c r="A227" s="1">
         <v>225</v>
       </c>
@@ -20853,7 +20829,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="228" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:27">
       <c r="A228" s="1">
         <v>226</v>
       </c>
@@ -20936,7 +20912,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="229" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:27">
       <c r="A229" s="1">
         <v>227</v>
       </c>
@@ -21019,7 +20995,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="230" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:27">
       <c r="A230" s="1">
         <v>228</v>
       </c>
@@ -21102,7 +21078,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="231" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:27">
       <c r="A231" s="1">
         <v>229</v>
       </c>
@@ -21185,7 +21161,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="232" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:27">
       <c r="A232" s="1">
         <v>230</v>
       </c>
@@ -21268,7 +21244,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="233" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:27">
       <c r="A233" s="1">
         <v>231</v>
       </c>
@@ -21351,7 +21327,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="234" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:27">
       <c r="A234" s="1">
         <v>232</v>
       </c>
@@ -21434,7 +21410,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="235" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:27">
       <c r="A235" s="1">
         <v>233</v>
       </c>
@@ -21517,7 +21493,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="236" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:27">
       <c r="A236" s="1">
         <v>234</v>
       </c>
@@ -21600,7 +21576,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="237" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:27">
       <c r="A237" s="1">
         <v>235</v>
       </c>
@@ -21683,7 +21659,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="238" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:27">
       <c r="A238" s="1">
         <v>236</v>
       </c>
@@ -21766,7 +21742,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="239" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:27">
       <c r="A239" s="1">
         <v>237</v>
       </c>
@@ -21849,7 +21825,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="240" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:27">
       <c r="A240" s="1">
         <v>238</v>
       </c>
@@ -21932,7 +21908,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="241" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:27">
       <c r="A241" s="1">
         <v>239</v>
       </c>
@@ -22015,7 +21991,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="242" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:27">
       <c r="A242" s="1">
         <v>240</v>
       </c>
@@ -22098,7 +22074,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="243" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:27">
       <c r="A243" s="1">
         <v>241</v>
       </c>
@@ -22181,7 +22157,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="244" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:27">
       <c r="A244" s="1">
         <v>242</v>
       </c>
@@ -22264,7 +22240,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="245" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:27">
       <c r="A245" s="1">
         <v>243</v>
       </c>
@@ -22347,7 +22323,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="246" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:27">
       <c r="A246" s="1">
         <v>244</v>
       </c>
@@ -22430,7 +22406,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="247" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:27">
       <c r="A247" s="1">
         <v>245</v>
       </c>
@@ -22513,7 +22489,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="248" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:27">
       <c r="A248" s="1">
         <v>246</v>
       </c>
@@ -22596,7 +22572,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="249" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:27">
       <c r="A249" s="1">
         <v>247</v>
       </c>
@@ -22679,7 +22655,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="250" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:27">
       <c r="A250" s="1">
         <v>248</v>
       </c>
@@ -22762,7 +22738,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="251" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:27">
       <c r="A251" s="1">
         <v>249</v>
       </c>
@@ -22845,7 +22821,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="252" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:27">
       <c r="A252" s="1">
         <v>250</v>
       </c>
@@ -22928,7 +22904,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="253" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:27">
       <c r="A253" s="1">
         <v>251</v>
       </c>
@@ -23011,7 +22987,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="254" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:27">
       <c r="A254" s="1">
         <v>252</v>
       </c>
@@ -23094,7 +23070,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="255" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:27">
       <c r="A255" s="1">
         <v>253</v>
       </c>
@@ -23177,7 +23153,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="256" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:27">
       <c r="A256" s="1">
         <v>254</v>
       </c>
@@ -23260,7 +23236,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="257" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:27">
       <c r="A257" s="1">
         <v>255</v>
       </c>
@@ -23343,7 +23319,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="258" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:27">
       <c r="A258" s="1">
         <v>256</v>
       </c>
@@ -23426,7 +23402,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="259" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:27">
       <c r="A259" s="1">
         <v>257</v>
       </c>
@@ -23509,7 +23485,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="260" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:27">
       <c r="A260" s="1">
         <v>258</v>
       </c>
@@ -23592,7 +23568,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="261" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:27">
       <c r="A261" s="1">
         <v>259</v>
       </c>
@@ -23675,7 +23651,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="262" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:27">
       <c r="A262" s="1">
         <v>260</v>
       </c>
@@ -23758,7 +23734,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="263" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:27">
       <c r="A263" s="1">
         <v>261</v>
       </c>
@@ -23841,7 +23817,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="264" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:27">
       <c r="A264" s="1">
         <v>262</v>
       </c>
@@ -23924,7 +23900,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="265" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:27">
       <c r="A265" s="1">
         <v>263</v>
       </c>
@@ -24007,7 +23983,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="266" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:27">
       <c r="A266" s="1">
         <v>264</v>
       </c>
@@ -24090,7 +24066,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="267" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:27">
       <c r="A267" s="1">
         <v>265</v>
       </c>
@@ -24173,7 +24149,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="268" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:27">
       <c r="A268" s="1">
         <v>266</v>
       </c>
@@ -24256,7 +24232,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="269" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:27">
       <c r="A269" s="1">
         <v>267</v>
       </c>
@@ -24339,7 +24315,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="270" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:27">
       <c r="A270" s="1">
         <v>268</v>
       </c>
@@ -24422,7 +24398,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="271" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:27">
       <c r="A271" s="1">
         <v>269</v>
       </c>
@@ -24505,7 +24481,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="272" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:27">
       <c r="A272" s="1">
         <v>270</v>
       </c>
@@ -24588,7 +24564,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="273" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:27">
       <c r="A273" s="1">
         <v>271</v>
       </c>
@@ -24671,7 +24647,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="274" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:27">
       <c r="A274" s="1">
         <v>272</v>
       </c>
@@ -24754,7 +24730,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="275" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:27">
       <c r="A275" s="1">
         <v>273</v>
       </c>
@@ -24837,7 +24813,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="276" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:27">
       <c r="A276" s="1">
         <v>274</v>
       </c>
@@ -24920,7 +24896,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="277" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:27">
       <c r="A277" s="1">
         <v>275</v>
       </c>
@@ -25003,7 +24979,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="278" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:27">
       <c r="A278" s="1">
         <v>276</v>
       </c>
@@ -25086,7 +25062,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="279" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:27">
       <c r="A279" s="1">
         <v>277</v>
       </c>
@@ -25169,7 +25145,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="280" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:27">
       <c r="A280" s="1">
         <v>278</v>
       </c>
@@ -25252,7 +25228,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="281" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:27">
       <c r="A281" s="1">
         <v>279</v>
       </c>
@@ -25335,7 +25311,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="282" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:27">
       <c r="A282" s="1">
         <v>280</v>
       </c>
@@ -25418,7 +25394,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="283" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:27">
       <c r="A283" s="1">
         <v>281</v>
       </c>
@@ -25501,7 +25477,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="284" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:27">
       <c r="A284" s="1">
         <v>282</v>
       </c>
@@ -25584,7 +25560,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="285" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:27">
       <c r="A285" s="1">
         <v>283</v>
       </c>
@@ -25667,7 +25643,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="286" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:27">
       <c r="A286" s="1">
         <v>284</v>
       </c>
@@ -25750,7 +25726,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="287" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:27">
       <c r="A287" s="1">
         <v>285</v>
       </c>
@@ -25833,7 +25809,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="288" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:27">
       <c r="A288" s="1">
         <v>286</v>
       </c>
@@ -25916,7 +25892,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="289" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:27">
       <c r="A289" s="1">
         <v>287</v>
       </c>
@@ -25999,7 +25975,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="290" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:27">
       <c r="A290" s="1">
         <v>288</v>
       </c>
@@ -26082,7 +26058,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="291" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:27">
       <c r="A291" s="1">
         <v>289</v>
       </c>
@@ -26165,7 +26141,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="292" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:27">
       <c r="A292" s="1">
         <v>290</v>
       </c>
@@ -26248,7 +26224,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="293" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:27">
       <c r="A293" s="1">
         <v>291</v>
       </c>
@@ -26331,7 +26307,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="294" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:27">
       <c r="A294" s="1">
         <v>292</v>
       </c>
@@ -26414,7 +26390,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="295" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:27">
       <c r="A295" s="1">
         <v>293</v>
       </c>
@@ -26497,7 +26473,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="296" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:27">
       <c r="A296" s="1">
         <v>294</v>
       </c>
@@ -26580,7 +26556,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="297" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:27">
       <c r="A297" s="1">
         <v>295</v>
       </c>
@@ -26663,7 +26639,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="298" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:27">
       <c r="A298" s="1">
         <v>296</v>
       </c>
@@ -26746,7 +26722,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="299" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:27">
       <c r="A299" s="1">
         <v>297</v>
       </c>
@@ -26829,7 +26805,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="300" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:27">
       <c r="A300" s="1">
         <v>298</v>
       </c>
@@ -26912,7 +26888,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="301" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:27">
       <c r="A301" s="1">
         <v>299</v>
       </c>
@@ -26995,7 +26971,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="302" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:27">
       <c r="A302" s="1">
         <v>300</v>
       </c>
@@ -27078,7 +27054,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="303" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:27">
       <c r="A303" s="1">
         <v>301</v>
       </c>
@@ -27161,7 +27137,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="304" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:27">
       <c r="A304" s="1">
         <v>302</v>
       </c>
@@ -27244,7 +27220,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="305" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:27">
       <c r="A305" s="1">
         <v>303</v>
       </c>
@@ -27327,7 +27303,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="306" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:27">
       <c r="A306" s="1">
         <v>304</v>
       </c>

</xml_diff>